<commit_message>
cissp d4 reading starts
</commit_message>
<xml_diff>
--- a/pyth26/L1-IPO-Sudo-Assignment.xlsx
+++ b/pyth26/L1-IPO-Sudo-Assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcchu\gitable2025\pyth26\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJCWKZ23\gitable2025\pyth26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68175048-8CCC-40A3-AD00-A89BBACBFE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB06BA9-EFB7-41E7-A8B5-068C27E1AE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1290" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D8A0ADC8-7A95-4E7A-B316-76A12385E8C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D8A0ADC8-7A95-4E7A-B316-76A12385E8C4}"/>
   </bookViews>
   <sheets>
     <sheet name="PB example" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="174">
   <si>
     <t>Input</t>
   </si>
@@ -172,24 +172,6 @@
     <t>Constants</t>
   </si>
   <si>
-    <t>Fried Rice = $10 =@Frice</t>
-  </si>
-  <si>
-    <t>Egg Roll = $2 = @Eroll</t>
-  </si>
-  <si>
-    <t>HotnSourSoup  = $3 = @HNSoup</t>
-  </si>
-  <si>
-    <t>menu = 1 / customer = 1</t>
-  </si>
-  <si>
-    <t>Part A - Restaurant order per customer  - IPO</t>
-  </si>
-  <si>
-    <t>Part A - Restaurant order per customer  - Psuedcode</t>
-  </si>
-  <si>
     <t>subtotal</t>
   </si>
   <si>
@@ -202,126 +184,36 @@
     <t>qual_@SFoodN</t>
   </si>
   <si>
-    <t>Seafood Noodle = $15 = @SFoodN</t>
-  </si>
-  <si>
     <t>qual_@HNSoup</t>
   </si>
   <si>
-    <t>tax rate= 8.5%</t>
-  </si>
-  <si>
     <t>BEGIN</t>
   </si>
   <si>
     <t>  // ----- Constants -----</t>
   </si>
   <si>
-    <t>  SET priceBurger = 5.00</t>
-  </si>
-  <si>
-    <t>  SET priceFries  = 2.50</t>
-  </si>
-  <si>
-    <t>  SET priceSoda   = 1.75</t>
-  </si>
-  <si>
-    <t>  SET taxRate     = 0.095         // 9.5% example</t>
-  </si>
-  <si>
     <t>  // ----- Display Menu -----</t>
   </si>
   <si>
-    <t>  PRINT "Welcome to QuickBite!"</t>
-  </si>
-  <si>
     <t>  PRINT "Menu:"</t>
   </si>
   <si>
-    <t>  PRINT "  1) Burger .... $5.00"</t>
-  </si>
-  <si>
-    <t>  PRINT "  2) Fries ..... $2.50"</t>
-  </si>
-  <si>
-    <t>  PRINT "  3) Soda ...... $1.75"</t>
-  </si>
-  <si>
-    <t>  // ----- Input Quantities -----</t>
-  </si>
-  <si>
     <t>  PRINT "Enter quantities (whole numbers)."</t>
   </si>
   <si>
-    <t>  INPUT qtyBurger</t>
-  </si>
-  <si>
-    <t>  INPUT qtyFries</t>
-  </si>
-  <si>
-    <t>  INPUT qtySoda</t>
-  </si>
-  <si>
-    <t>  // ----- Basic Validation -----</t>
-  </si>
-  <si>
-    <t>  IF qtyBurger &lt; 0 OR qtyFries &lt; 0 OR qtySoda &lt; 0 THEN</t>
-  </si>
-  <si>
-    <t>      PRINT "Error: Quantities cannot be negative."</t>
-  </si>
-  <si>
     <t>      EXIT PROGRAM</t>
   </si>
   <si>
-    <t>  ENDIF</t>
-  </si>
-  <si>
-    <t>  // Optionally ensure integers:</t>
-  </si>
-  <si>
-    <t>  // IF any qty is not an integer THEN error and EXIT</t>
-  </si>
-  <si>
     <t>  // ----- Calculations -----</t>
   </si>
   <si>
-    <t>  SET lineBurger = qtyBurger * priceBurger</t>
-  </si>
-  <si>
-    <t>  SET lineFries  = qtyFries  * priceFries</t>
-  </si>
-  <si>
-    <t>  SET lineSoda   = qtySoda   * priceSoda</t>
-  </si>
-  <si>
-    <t>  SET subtotal = lineBurger + lineFries + lineSoda</t>
-  </si>
-  <si>
-    <t>  SET tax      = subtotal * taxRate</t>
-  </si>
-  <si>
-    <t>  SET total    = subtotal + tax</t>
-  </si>
-  <si>
     <t>  // ----- Output Receipt -----</t>
   </si>
   <si>
     <t>  PRINT "-----------------------------"</t>
   </si>
   <si>
-    <t>  PRINT "           RECEIPT"</t>
-  </si>
-  <si>
-    <t>  PRINT "Burger x " + qtyBurger + " @ $" + priceBurger + " = $" + FORMAT(lineBurger, 2)</t>
-  </si>
-  <si>
-    <t>  PRINT "Fries  x " + qtyFries  + " @ $" + priceFries  + " = $" + FORMAT(lineFries, 2)</t>
-  </si>
-  <si>
-    <t>  PRINT "Soda   x " + qtySoda   + " @ $" + priceSoda   + " = $" + FORMAT(lineSoda, 2)</t>
-  </si>
-  <si>
     <t>  PRINT "Subtotal: $" + FORMAT(subtotal, 2)</t>
   </si>
   <si>
@@ -335,13 +227,343 @@
   </si>
   <si>
     <t>END</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>menu = 1 data list which contains food items and prices</t>
+  </si>
+  <si>
+    <t>Menu data list is copied or</t>
+  </si>
+  <si>
+    <t>Insert menu data list into the customer_input memory space</t>
+  </si>
+  <si>
+    <t>read into customer_input</t>
+  </si>
+  <si>
+    <t>Customer_input</t>
+  </si>
+  <si>
+    <t>Processing on customer_input by insert that</t>
+  </si>
+  <si>
+    <t>into another external function called</t>
+  </si>
+  <si>
+    <t>(what he/she wants to order)</t>
+  </si>
+  <si>
+    <t>iDecision_process then produce output… what to order</t>
+  </si>
+  <si>
+    <t>customer_decision</t>
+  </si>
+  <si>
+    <t>customer_decison</t>
+  </si>
+  <si>
+    <t>Processing on customer_decision by insert that</t>
+  </si>
+  <si>
+    <t>qual_@  values filled</t>
+  </si>
+  <si>
+    <t>(qty he/she wants to order)</t>
+  </si>
+  <si>
+    <t>qual_values with their according prices listed in the menu</t>
+  </si>
+  <si>
+    <t>Calculuate the subtotal by multiplying each</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subtotal </t>
+  </si>
+  <si>
+    <t>f-price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate the final price by multiplying </t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_tax= +8.5% =1.085 </t>
+  </si>
+  <si>
+    <t>add_tax</t>
+  </si>
+  <si>
+    <t>subtotal by add_tax</t>
+  </si>
+  <si>
+    <t>print order summary</t>
+  </si>
+  <si>
+    <t>subtotal \ f-price \ invoice</t>
+  </si>
+  <si>
+    <t>customer_input \customer_decision</t>
+  </si>
+  <si>
+    <t>  PRINT "Welcome to Lucky Cafe!"</t>
+  </si>
+  <si>
+    <t>  PRINT "  1) Frice Rice .... $10.00"</t>
+  </si>
+  <si>
+    <t>  PRINT "  2) Egg Roll ..... $2.00"</t>
+  </si>
+  <si>
+    <t>  PRINT "  3) Seafood Noodle...... $17.75"</t>
+  </si>
+  <si>
+    <t>  PRINT "  4)  Hot n Sour Soup...... $3.00"</t>
+  </si>
+  <si>
+    <t>iDeceision_process.qty.qual_@Frice = qual_@Frice</t>
+  </si>
+  <si>
+    <t>  // ----- Calling external function to obtain what and qty wanted order -----</t>
+  </si>
+  <si>
+    <t>iDeceision_process.qty.qual_@Eroll = qual_@Eroll</t>
+  </si>
+  <si>
+    <t>iDeceision_process.qty.qual_@SFoodN = qual_@SFoodN</t>
+  </si>
+  <si>
+    <t>iDeceision_process.qty.qual_@HNSoup =qual_@HNSoup</t>
+  </si>
+  <si>
+    <t>  INPUT qual_@Frice</t>
+  </si>
+  <si>
+    <t>  INPUT qual_@Eroll</t>
+  </si>
+  <si>
+    <t>  INPUT qual_@SFoodN</t>
+  </si>
+  <si>
+    <t>  INPUT qual_@HNSoup</t>
+  </si>
+  <si>
+    <t>  // ----- input and basic less-than-zero and non-integer validation -----</t>
+  </si>
+  <si>
+    <t>  SET subtotal = lineFRice + lineEroll  + lineSFoodN  + lineHNSoup  </t>
+  </si>
+  <si>
+    <t>  SET tax      = subtotal * 0.085</t>
+  </si>
+  <si>
+    <t>  SET total    = subtotal * add_tax</t>
+  </si>
+  <si>
+    <t>  PRINT "           ORDER SUMMARY FROM LUCY CAFÉ … THANK YOU!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK LIB iDeceision_process </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //---external ai decision making library to simulate a customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF (qual_@Frice &lt; 0 OR qual_@Eroll &lt; 0 OR  qual_@SFoodN &lt; 0  OR qual_@HNSoup &lt; 0 ) </t>
+  </si>
+  <si>
+    <t>ELSE IF (qual_@Frice OR qual_@Eroll OR  qual_@SFoodN OR qual_@HNSoup ) != INTEGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      PRINT "Error: Quantities cannot be negative"</t>
+  </si>
+  <si>
+    <t>      PRINT "Error: Quantities cannot be non-integer"</t>
+  </si>
+  <si>
+    <t>ENDIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invoice / Receipt </t>
+  </si>
+  <si>
+    <t>Part A - Movie Theater  - IPO</t>
+  </si>
+  <si>
+    <t>Part A - Restaurant order  - IPO</t>
+  </si>
+  <si>
+    <t>Part A - Restaurant order - Psuedcode</t>
+  </si>
+  <si>
+    <t>Adult = $18</t>
+  </si>
+  <si>
+    <t>Student = $12</t>
+  </si>
+  <si>
+    <t>Child = $8</t>
+  </si>
+  <si>
+    <t>adult_qty</t>
+  </si>
+  <si>
+    <t>Student_qty</t>
+  </si>
+  <si>
+    <t>Child_qty</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Constants: Adult, Student, Child</t>
+  </si>
+  <si>
+    <t>Print out constants as a menu , list out each prices for Adult, Student, Child</t>
+  </si>
+  <si>
+    <t>adult_qty, student_qty, child_qty</t>
+  </si>
+  <si>
+    <t>variables set with new values from the default</t>
+  </si>
+  <si>
+    <t>costants for adult,student,child</t>
+  </si>
+  <si>
+    <t>calcuate the subtotal with values of the qty and constants/prices</t>
+  </si>
+  <si>
+    <t>calculate the total by multiplying the subtotal with the add_tax</t>
+  </si>
+  <si>
+    <t>subtotal / tax added / total</t>
+  </si>
+  <si>
+    <t>accepting input and insert values entered into the variables … with some basic vaildations</t>
+  </si>
+  <si>
+    <t>HNSoup = 3</t>
+  </si>
+  <si>
+    <t>SFoodN = 17.75</t>
+  </si>
+  <si>
+    <t>Eroll = 2</t>
+  </si>
+  <si>
+    <t>Frice = 10</t>
+  </si>
+  <si>
+    <t>  SET lineFRice = qual_@Frice * Frice</t>
+  </si>
+  <si>
+    <t>  SET lineEroll  = qual_@Eroll * Eroll</t>
+  </si>
+  <si>
+    <t>  SET lineSFoodN   = qual_@SFoodN * SFoodN</t>
+  </si>
+  <si>
+    <t>  SET lineHNSoup   = qual_@HNSoup * HNSoup</t>
+  </si>
+  <si>
+    <t>  PRINT "Fried Rice  X " + qual_@Frice + " @ $" + Frice + " = $" + FORMAT(lineFRice, 2)</t>
+  </si>
+  <si>
+    <t>  PRINT "Egg Roll   X " +  qual_@Eroll + " @ $" + Eroll + " = $" + FORMAT(lineEroll, 2)</t>
+  </si>
+  <si>
+    <t>  PRINT "Seafood Noodle   X " +  qual_@SFoodN + " @ $" + SFoodN + " = $" + FORMAT(  SET lineSFoodN, 2)</t>
+  </si>
+  <si>
+    <t>  PRINT "HotnSour Soup  X " + qual_@HNSoup + " @ $" + HNSoup + " = $" + FORMAT( SET lineHNSoup, 2)</t>
+  </si>
+  <si>
+    <t>Fried Rice = $10 =Frice</t>
+  </si>
+  <si>
+    <t>Egg Roll = $2 = Eroll</t>
+  </si>
+  <si>
+    <t>Seafood Noodle = $17.75 = SFoodN</t>
+  </si>
+  <si>
+    <t>HotnSourSoup  = $3 = HNSoup</t>
+  </si>
+  <si>
+    <t>constants item price values</t>
+  </si>
+  <si>
+    <t>Adult = 18</t>
+  </si>
+  <si>
+    <t>Student = 12</t>
+  </si>
+  <si>
+    <t>Child = 8</t>
+  </si>
+  <si>
+    <t>tax_rate = 0.085</t>
+  </si>
+  <si>
+    <t>  PRINT "  1) Each ADULT ticket is .... $10.00"</t>
+  </si>
+  <si>
+    <t>  PRINT "  2) Each ADULT ticket is ..... $2.00"</t>
+  </si>
+  <si>
+    <t>  PRINT "  3) Each CHILD ticket is...... $17.75"</t>
+  </si>
+  <si>
+    <t>  PRINT "           The Order Summary from YOUR Neon Marquee Theater… THANK YOU!"</t>
+  </si>
+  <si>
+    <t>adult_qty=Print (INPUT(INT("Enter the Qty of ADULT tickets you want:   ")))</t>
+  </si>
+  <si>
+    <t>student_qty=Print (INPUT(INT("Enter the Qty of STUDENT tickets you want:   ")))</t>
+  </si>
+  <si>
+    <t>child_qty=Print (INPUT(INT("Enter the Qty of CHILD tickets you want:   ")))</t>
+  </si>
+  <si>
+    <t>  SET totaladult = adult_qty * Adult</t>
+  </si>
+  <si>
+    <t>  SET totalstudent = student_qty * Student</t>
+  </si>
+  <si>
+    <t>  SET totalchild = child_qty * Child</t>
+  </si>
+  <si>
+    <t>  SET subtotal = totaladult + totalstudent + totalchild</t>
+  </si>
+  <si>
+    <t>  PRINT "Adult tickets  X " + adult_qty + " @ $" + Adult + " = $" + FORMAT(totaladult, 2)</t>
+  </si>
+  <si>
+    <t>  PRINT "Student tickets  X " + student_qty + " @ $" + Student + " = $" + FORMAT(totalstudent, 2)</t>
+  </si>
+  <si>
+    <t>  PRINT "Child tickets  X " + child_qty + " @ $" + Child + " = $" + FORMAT(totalchild, 2)</t>
+  </si>
+  <si>
+    <t>  PRINT "Thank you for your business !"</t>
+  </si>
+  <si>
+    <t>Part A - Movie Theate - Psuedcode</t>
+  </si>
+  <si>
+    <t>print menu waiting for qty to be input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,8 +609,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,8 +629,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -634,12 +868,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -652,24 +925,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -696,12 +951,75 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -727,13 +1045,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>29607</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5067300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>11072</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -756,8 +1074,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="723899"/>
-          <a:ext cx="10658475" cy="5830333"/>
+          <a:off x="0" y="647700"/>
+          <a:ext cx="12620625" cy="6011822"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1130,16 +1448,16 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="27">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="30" t="s">
         <v>10</v>
       </c>
       <c r="H9" t="s">
@@ -1147,23 +1465,23 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="12"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="31"/>
       <c r="H10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="32"/>
       <c r="G11">
         <v>1</v>
       </c>
@@ -1192,10 +1510,10 @@
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="27" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="s">
@@ -1206,8 +1524,8 @@
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
       <c r="H14" t="s">
         <v>31</v>
       </c>
@@ -1216,8 +1534,8 @@
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
       <c r="G15">
         <v>3</v>
       </c>
@@ -1272,7 +1590,7 @@
       <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="27" t="s">
         <v>24</v>
       </c>
       <c r="G19">
@@ -1289,7 +1607,7 @@
       <c r="C20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="9"/>
+      <c r="D20" s="28"/>
       <c r="H20" t="s">
         <v>38</v>
       </c>
@@ -1301,7 +1619,7 @@
       <c r="C21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="29"/>
       <c r="H21" t="s">
         <v>33</v>
       </c>
@@ -1337,12 +1655,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D19:D21"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1352,402 +1670,849 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846886B9-5465-4EFA-9FF3-8FFD41324B46}">
-  <dimension ref="B2:X59"/>
+  <dimension ref="A2:M81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.85546875" customWidth="1"/>
-    <col min="21" max="21" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1"/>
-    <col min="24" max="24" width="77.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="78.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" customWidth="1"/>
+    <col min="10" max="10" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="97" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="T5" s="17" t="s">
+    <row r="5" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="I5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I8" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I9" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I10" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I11" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="X5" s="17" t="s">
+      <c r="J11" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="M11" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="M12" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I14" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I15" s="35"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="M15" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I16" s="40"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="42"/>
+      <c r="M16" s="25"/>
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I18" s="15"/>
+      <c r="J18" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="M18" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="17"/>
+      <c r="J19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19" s="19"/>
+      <c r="M19" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="M20" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I21" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="M21" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="35"/>
+      <c r="J22" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="K22" s="43"/>
+      <c r="M22" s="25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I24" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K24" s="16"/>
+      <c r="M24" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="17"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="19"/>
+      <c r="M25" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="I26" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="J26" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="K26" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="M26" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I27" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="J27" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="K27" s="39"/>
+      <c r="M27" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I28" s="45"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="39"/>
+      <c r="M28" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J29" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="K29" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="M29" s="25"/>
+    </row>
+    <row r="30" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I30" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J30" s="46"/>
+      <c r="K30" s="47"/>
+      <c r="M30" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J31" s="46"/>
+      <c r="K31" s="47"/>
+      <c r="M31" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J32" s="46"/>
+      <c r="K32" s="47"/>
+      <c r="M32" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M35" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B36" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="H36" s="11"/>
+      <c r="M36" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="H37" s="11"/>
+      <c r="M37" s="48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="11"/>
+      <c r="M38" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B39" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="24" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T7" s="6" t="s">
+      <c r="H39" s="11"/>
+      <c r="M39" s="48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B40" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" s="25"/>
+      <c r="H40" s="11"/>
+      <c r="M40" s="25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B41" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F41" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="H41" s="11"/>
+      <c r="M41" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B42" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="H42" s="11"/>
+      <c r="M42" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="F43" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="H43" s="11"/>
+      <c r="M43" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H44" s="11"/>
+      <c r="M44" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="H45" s="11"/>
+      <c r="M45" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B46" s="35"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="F46" s="25"/>
+      <c r="H46" s="11"/>
+      <c r="M46" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="40"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="F47" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="11"/>
+      <c r="M47" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="M48" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="15"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="F49" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M49" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="17"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="52"/>
+      <c r="F50" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="M50" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="M51" s="25"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="F52" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="M52" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="X7" s="31" t="s">
+    </row>
+    <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="17"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="52"/>
+      <c r="F53" s="25"/>
+      <c r="M53" s="25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T8" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="X8" s="32"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T9" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="U9" s="6" t="s">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>4</v>
+      </c>
+      <c r="B54" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="X9" s="32" t="s">
+      <c r="C54" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="F54" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="M54" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
+      <c r="F55" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="M55" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="17"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="F56" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="M56" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
+      <c r="F57" s="25"/>
+      <c r="M57" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
+      <c r="F58" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="M58" s="25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="F59" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="M59" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F60" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="M60" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F61" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="M61" s="25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T10" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="X10" s="32" t="s">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F62" s="25"/>
+      <c r="M62" s="25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T11" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="U11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="X11" s="32" t="s">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F63" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="M63" s="25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S12" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="X12" s="32" t="s">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F64" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="M64" s="25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S13">
-        <v>1</v>
-      </c>
-      <c r="T13" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="U13" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="V13" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="X13" s="32" t="s">
+    <row r="65" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F65" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="M65" s="25"/>
+    </row>
+    <row r="66" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F66" s="25"/>
+      <c r="M66" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T14" s="21"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="20"/>
-      <c r="X14" s="32"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T15" s="21"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="22"/>
-      <c r="X15" s="32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T16" s="23"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="25"/>
-      <c r="X16" s="32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="S17">
-        <v>2</v>
-      </c>
-      <c r="T17" s="18"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="20"/>
-      <c r="X17" s="32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="T18" s="21"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="22"/>
-      <c r="X18" s="32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="19:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T19" s="23"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="25"/>
-      <c r="X19" s="32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="S20">
-        <v>3</v>
-      </c>
-      <c r="T20" s="18"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="20"/>
-      <c r="X20" s="32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="T21" s="21"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="22"/>
-      <c r="X21" s="32"/>
-    </row>
-    <row r="22" spans="19:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T22" s="23"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="25"/>
-      <c r="X22" s="32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="S23">
-        <v>4</v>
-      </c>
-      <c r="T23" s="18"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="20"/>
-      <c r="X23" s="32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="T24" s="21"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="22"/>
-      <c r="X24" s="32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="19:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T25" s="23"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="25"/>
-      <c r="X25" s="32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="S26">
-        <v>5</v>
-      </c>
-      <c r="T26" s="18"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="20"/>
-      <c r="X26" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="T27" s="21"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="22"/>
-      <c r="X27" s="32"/>
-    </row>
-    <row r="28" spans="19:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T28" s="23"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="25"/>
-      <c r="X28" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="X29" s="32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="X30" s="32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="X31" s="32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="X32" s="32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X33" s="32"/>
-    </row>
-    <row r="34" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X34" s="32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X35" s="32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X36" s="32"/>
-    </row>
-    <row r="37" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X37" s="32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X38" s="32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X39" s="32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X40" s="32" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X41" s="32"/>
-    </row>
-    <row r="42" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X42" s="32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X43" s="32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X44" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X45" s="32"/>
-    </row>
-    <row r="46" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X46" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X47" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X48" s="32" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X49" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X50" s="32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X51" s="32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X52" s="32" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X53" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X54" s="32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X55" s="32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X56" s="32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X57" s="32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X58" s="32"/>
-    </row>
-    <row r="59" spans="24:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="X59" s="33" t="s">
-        <v>99</v>
+    <row r="67" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F67" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F68" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F69" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F70" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F71" s="25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F72" s="25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F73" s="25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F74" s="25"/>
+    </row>
+    <row r="75" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F75" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F76" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F77" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F78" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F79" s="25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F80" s="25"/>
+    </row>
+    <row r="81" spans="6:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F81" s="26" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="D57:D59"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{740AD086-D85A-4DE4-92CA-76971BAC002A}"/>
+    <hyperlink ref="K20" r:id="rId2" xr:uid="{1F45DFE9-1E40-4341-B6F2-539E33D5AADA}"/>
+    <hyperlink ref="I23" r:id="rId3" xr:uid="{0C95C1F2-711C-4AB2-9189-355D8AD5C8ED}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{E44D9A0F-1210-4A65-9067-43B8A7427BDF}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{5B507388-84C4-4365-A1CC-2F5043369812}"/>
+    <hyperlink ref="I10" r:id="rId6" xr:uid="{070B40C2-3C53-4648-A0DD-7D1AABC0440D}"/>
+    <hyperlink ref="I11" r:id="rId7" xr:uid="{D827D686-376E-4DC5-AC3B-98720460BA8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>